<commit_message>
Fixed recording game time
</commit_message>
<xml_diff>
--- a/game_data.xlsx
+++ b/game_data.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -415,8 +414,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -461,7 +460,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>agent_minimax</t>
+          <t>agent_random</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -474,12 +473,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>agent_minimax</t>
+          <t>agent_random</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.029</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -489,13 +488,13 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2 2 0 0 0 0
-2 0 0 0 0 0
-0 0 0 0 0 0
-1 1 1 1 0 0
-2 1 0 0 0 0
-0 0 0 0 0 0
-2 1 0 0 0 0</t>
+          <t>2 1 2 0 0 0
+1 2 0 0 0 0
+2 1 1 0 0 0
+2 1 1 0 0 0
+2 1 2 0 0 0
+1 1 0 0 0 0
+1 2 2 0 0 0</t>
         </is>
       </c>
     </row>
@@ -511,7 +510,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -520,7 +519,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.0426</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -530,13 +529,13 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2 0 0 0 0 0
+          <t>1 2 2 0 0 0
+0 0 0 0 0 0
+2 1 1 1 1 0
+1 2 1 2 1 2
 2 1 0 0 0 0
-2 0 0 0 0 0
-2 1 0 0 0 0
-1 2 1 1 2 1
-1 2 2 0 0 0
-1 0 0 0 0 0</t>
+2 2 0 0 0 0
+1 1 2 1 2 0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added new block fork heuristic
</commit_message>
<xml_diff>
--- a/game_data.xlsx
+++ b/game_data.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,10 +413,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -456,11 +457,16 @@
           <t>Final Board</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Depth</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>agent_random</t>
+          <t>agent_minimax</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -473,12 +479,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>agent_random</t>
+          <t>agent_minimax</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.029</t>
+          <t>0.4764</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -489,19 +495,22 @@
       <c r="G2" t="inlineStr">
         <is>
           <t>2 1 2 0 0 0
-1 2 0 0 0 0
-2 1 1 0 0 0
-2 1 1 0 0 0
-2 1 2 0 0 0
+2 2 1 2 1 0
+2 0 0 0 0 0
 1 1 0 0 0 0
-1 2 2 0 0 0</t>
-        </is>
+1 1 0 0 0 0
+2 1 0 0 0 0
+2 1 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>agent_random</t>
+          <t>agent_minimax</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -514,29 +523,296 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.3965</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1 2 0 0 0 0
+0 0 0 0 0 0
+1 0 0 0 0 0
+1 2 2 0 0 0
+1 0 0 0 0 0
+1 2 0 0 0 0
+0 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2.4856</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1 1 2 2 0 0
+2 2 2 1 1 2
+2 1 1 2 1 2
+1 2 1 2 2 1
+2 1 1 2 2 1
+1 1 2 1 2 1
+1 1 2 2 0 0</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.6667</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2 1 2 0 0 0
+2 1 2 2 1 1
+1 2 1 2 2 1
+1 1 2 2 1 2
+1 1 0 0 0 0
+2 2 1 0 0 0
+2 1 1 2 1 2</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1.6489</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1 1 1 2 2 0
+1 1 2 0 0 0
+2 2 2 1 2 1
+1 1 2 1 2 2
+1 1 2 1 2 0
+2 0 0 0 0 0
+0 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>7.3418</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1 1 1 2 1 0
+2 0 0 0 0 0
+2 2 2 1 1 0
+1 2 2 1 2 2
+1 2 0 0 0 0
+2 2 1 1 2 0
+1 1 1 2 1 2</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>agent_random</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0.0426</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>h_center_control|h_sliding_windows</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1 2 2 0 0 0
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.5217</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0 0 0 0 0 0
+2 0 0 0 0 0
+2 2 0 0 0 0
+1 1 1 1 0 0
+1 0 0 0 0 0
+2 0 0 0 0 0
+0 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>agent_random</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.2982</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1 0 0 0 0 0
+2 0 0 0 0 0
 0 0 0 0 0 0
-2 1 1 1 1 0
-1 2 1 2 1 2
-2 1 0 0 0 0
-2 2 0 0 0 0
-1 1 2 1 2 0</t>
-        </is>
+1 1 1 1 0 0
+2 0 0 0 0 0
+2 2 1 2 0 0
+1 2 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented offensive and defensive heuristics
</commit_message>
<xml_diff>
--- a/game_data.xlsx
+++ b/game_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,6 +815,534 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>agent_random</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>agent_random</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>17.1794</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2 1 1 0 0 0
+1 1 2 1 0 0
+2 2 2 0 0 0
+1 1 2 2 1 0
+2 1 2 2 0 0
+1 2 2 1 1 0
+1 2 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>agent_random</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>8.4680</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2 1 2 1 2 0
+0 0 0 0 0 0
+2 1 1 1 1 0
+1 2 1 2 0 0
+2 0 0 0 0 0
+2 1 2 1 2 0
+1 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>9.1750</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1 2 0 0 0 0
+1 2 0 0 0 0
+2 2 0 0 0 0
+1 2 1 0 0 0
+1 0 0 0 0 0
+0 0 0 0 0 0
+0 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>7.4280</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2 0 0 0 0 0
+1 2 2 0 0 0
+1 1 2 0 0 0
+1 1 1 2 0 0
+2 0 0 0 0 0
+0 0 0 0 0 0
+0 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>16.1865</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2 1 0 0 0 0
+1 2 0 0 0 0
+2 1 1 1 1 0
+1 2 2 0 0 0
+2 0 0 0 0 0
+1 2 0 0 0 0
+2 1 2 1 0 0</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>15.8501</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2 1 2 2 1 2
+1 1 1 2 1 2
+1 0 0 0 0 0
+1 2 2 1 2 1
+2 1 1 1 2 1
+2 1 0 0 0 0
+1 2 2 2 1 2</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12.5153</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2 2 1 2 0 0
+1 0 0 0 0 0
+2 1 1 1 2 0
+1 2 1 2 1 2
+1 1 2 0 0 0
+2 1 2 2 2 1
+1 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>agent_user</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>agent_user</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>61.7931</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2 0 0 0 0 0
+2 1 2 0 0 0
+1 2 1 2 0 0
+1 2 1 1 2 0
+1 1 2 1 1 0
+2 0 0 0 0 0
+0 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>7.0454</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2 0 0 0 0 0
+2 2 1 0 0 0
+2 1 2 0 0 0
+1 1 1 2 0 0
+2 2 1 0 0 0
+1 1 2 1 0 0
+0 0 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3.5081</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0 0 0 0 0 0
+2 1 1 2 2 0
+1 0 0 0 0 0
+1 1 2 0 0 0
+2 1 0 0 0 0
+2 1 0 0 0 0
+2 1 0 0 0 0</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>9.7790</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1 2 2 2 1 2
+1 1 2 0 0 0
+2 1 2 0 0 0
+1 1 2 0 0 0
+1 2 2 1 2 0
+2 2 1 2 0 0
+1 1 2 1 1 1</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>agent_minimax</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>16.7147</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>h_block_fork|h_center_control</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1 1 2 2 1 2
+2 1 2 0 0 0
+2 2 1 2 1 1
+1 2 1 2 2 2
+1 1 1 2 1 2
+2 0 0 0 0 0
+1 2 1 1 2 1</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>